<commit_message>
Neural Net Design Changes
- Add bias node to node map
- Update Record of Progress
- Update Revised Gantt Chart
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -281,8 +281,12 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -381,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -425,6 +429,8 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -468,6 +474,8 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,7 +808,7 @@
   <dimension ref="A1:BJ55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1083,19 +1091,20 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
     </row>
     <row r="10" spans="1:62">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:62">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:62">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Panel Implementation and Testing
- Create CSPanel class which acts as a canvas to be drawn on.
- Test Frame and Panel with driver code block
- Update Test Plan
- Update Record of progress
- Update Revised Gantt Chart
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <r>
       <rPr>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">    Pseudocode &amp; Class Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Frame and Panel</t>
   </si>
 </sst>
 </file>
@@ -287,8 +290,14 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -423,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -485,6 +494,9 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -546,6 +558,9 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -875,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ55"/>
+  <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AD21" sqref="AD21"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1190,6 +1205,7 @@
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
     </row>
     <row r="14" spans="1:62">
       <c r="A14" t="s">
@@ -1200,7 +1216,6 @@
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="T15" s="4"/>
       <c r="U15" s="4"/>
     </row>
     <row r="16" spans="1:62">
@@ -1261,204 +1276,210 @@
     </row>
     <row r="24" spans="1:38">
       <c r="A24" t="s">
-        <v>35</v>
-      </c>
-      <c r="L24" s="4"/>
-      <c r="AE24" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="T24" s="4"/>
     </row>
     <row r="25" spans="1:38">
       <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF25" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="L25" s="4"/>
+      <c r="AE25" s="4"/>
     </row>
     <row r="26" spans="1:38">
       <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG26" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="AF26" s="4"/>
     </row>
     <row r="27" spans="1:38">
       <c r="A27" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH27" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="AG27" s="4"/>
     </row>
     <row r="28" spans="1:38">
       <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI28" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="1:38">
       <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="AJ29" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="AI29" s="4"/>
     </row>
     <row r="30" spans="1:38">
       <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK30" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="AJ30" s="4"/>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="AL31" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="AK31" s="4"/>
     </row>
     <row r="32" spans="1:38">
       <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="AL32" s="4"/>
+    </row>
+    <row r="33" spans="1:59">
+      <c r="A33" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:60">
-      <c r="A33" t="s">
+    <row r="34" spans="1:59">
+      <c r="A34" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:60">
-      <c r="A34" t="s">
+    <row r="35" spans="1:59">
+      <c r="A35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:60">
-      <c r="A35" t="s">
+    <row r="36" spans="1:59">
+      <c r="A36" t="s">
         <v>29</v>
       </c>
-      <c r="AM35" s="4"/>
-      <c r="AN35" s="4"/>
-    </row>
-    <row r="36" spans="1:60">
-      <c r="A36" t="s">
+      <c r="AM36" s="4"/>
+      <c r="AN36" s="4"/>
+    </row>
+    <row r="37" spans="1:59">
+      <c r="A37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:60">
-      <c r="A37" t="s">
+    <row r="38" spans="1:59">
+      <c r="A38" t="s">
         <v>16</v>
-      </c>
-      <c r="AO37" s="4"/>
-      <c r="AP37" s="4"/>
-    </row>
-    <row r="38" spans="1:60">
-      <c r="A38" t="s">
-        <v>17</v>
       </c>
       <c r="AO38" s="4"/>
       <c r="AP38" s="4"/>
     </row>
-    <row r="39" spans="1:60">
+    <row r="39" spans="1:59">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AO39" s="4"/>
       <c r="AP39" s="4"/>
     </row>
-    <row r="40" spans="1:60">
+    <row r="40" spans="1:59">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AO40" s="4"/>
       <c r="AP40" s="4"/>
     </row>
-    <row r="41" spans="1:60">
+    <row r="41" spans="1:59">
       <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO41" s="4"/>
+      <c r="AP41" s="4"/>
+    </row>
+    <row r="42" spans="1:59">
+      <c r="A42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:60">
-      <c r="A42" t="s">
+    <row r="43" spans="1:59">
+      <c r="A43" t="s">
         <v>49</v>
       </c>
-      <c r="AQ42" s="4"/>
-      <c r="AR42" s="4"/>
-    </row>
-    <row r="43" spans="1:60">
-      <c r="A43" t="s">
+      <c r="AQ43" s="4"/>
+      <c r="AR43" s="4"/>
+    </row>
+    <row r="44" spans="1:59">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
-      <c r="AS43" s="4"/>
-      <c r="AT43" s="4"/>
-      <c r="AU43" s="4"/>
-      <c r="AV43" s="4"/>
-    </row>
-    <row r="44" spans="1:60">
-      <c r="A44" t="s">
+      <c r="AS44" s="4"/>
+      <c r="AT44" s="4"/>
+      <c r="AU44" s="4"/>
+      <c r="AV44" s="4"/>
+    </row>
+    <row r="45" spans="1:59">
+      <c r="A45" t="s">
         <v>22</v>
       </c>
-      <c r="AW44" s="4"/>
-      <c r="AX44" s="4"/>
-      <c r="AY44" s="4"/>
-      <c r="AZ44" s="4"/>
-      <c r="BA44" s="4"/>
-      <c r="BB44" s="4"/>
-      <c r="BC44" s="4"/>
-      <c r="BD44" s="4"/>
-      <c r="BE44" s="4"/>
-      <c r="BF44" s="4"/>
-    </row>
-    <row r="45" spans="1:60">
-      <c r="A45" t="s">
+      <c r="AW45" s="4"/>
+      <c r="AX45" s="4"/>
+      <c r="AY45" s="4"/>
+      <c r="AZ45" s="4"/>
+      <c r="BA45" s="4"/>
+      <c r="BB45" s="4"/>
+      <c r="BC45" s="4"/>
+      <c r="BD45" s="4"/>
+      <c r="BE45" s="4"/>
+      <c r="BF45" s="4"/>
+    </row>
+    <row r="46" spans="1:59">
+      <c r="A46" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:60">
-      <c r="A46" t="s">
+    <row r="47" spans="1:59">
+      <c r="A47" t="s">
         <v>23</v>
       </c>
-      <c r="BG46" s="4"/>
-    </row>
-    <row r="47" spans="1:60">
-      <c r="A47" t="s">
+      <c r="BG47" s="4"/>
+    </row>
+    <row r="48" spans="1:59">
+      <c r="A48" t="s">
         <v>20</v>
       </c>
-      <c r="BG47" s="4"/>
-    </row>
-    <row r="48" spans="1:60">
-      <c r="A48" t="s">
-        <v>21</v>
-      </c>
-      <c r="BH48" s="4"/>
+      <c r="BG48" s="4"/>
     </row>
     <row r="49" spans="1:62">
       <c r="A49" t="s">
-        <v>24</v>
-      </c>
-      <c r="BI49" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="BH49" s="4"/>
     </row>
     <row r="50" spans="1:62">
       <c r="A50" t="s">
-        <v>27</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="BI50" s="4"/>
     </row>
     <row r="51" spans="1:62">
       <c r="A51" t="s">
-        <v>16</v>
-      </c>
-      <c r="BJ51" s="4"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="52" spans="1:62">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="BJ52" s="4"/>
     </row>
     <row r="53" spans="1:62">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BJ53" s="4"/>
     </row>
     <row r="54" spans="1:62">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="BJ54" s="4"/>
     </row>
     <row r="55" spans="1:62">
       <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ55" s="4"/>
+    </row>
+    <row r="56" spans="1:62">
+      <c r="A56" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Full Neural Net Implementation
- Create and test HardlimNode class
- Create and test TanhNode class
- Modify SigmoidNode to be able to generate negative weights
- Update record of proress
- Update revised gantt chart
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -213,7 +213,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,8 +257,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +276,12 @@
       <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -290,7 +303,7 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -434,8 +447,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -445,8 +476,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -518,6 +550,15 @@
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -589,6 +630,15 @@
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,7 +971,7 @@
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1241,6 +1291,9 @@
       </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
     </row>
     <row r="15" spans="1:62">
       <c r="A15" t="s">
@@ -1251,8 +1304,6 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:38">
       <c r="A17" t="s">
@@ -1320,6 +1371,10 @@
       <c r="A26" t="s">
         <v>35</v>
       </c>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="4"/>
       <c r="AF26" s="4"/>
     </row>
     <row r="27" spans="1:38">

</xml_diff>

<commit_message>
CardLayout panel and switching between gamestates
- Change CSPanel to use the CardLayout layout, to enable switching between menus
- Create MainMenu and InGame panels
- Update record of progress
- Update revised gantt chart
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -303,8 +303,30 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="161">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -478,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="161">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -559,6 +581,17 @@
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -639,6 +672,17 @@
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -971,7 +1015,7 @@
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+      <selection activeCell="Z15" sqref="Z15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1299,6 +1343,8 @@
       <c r="A15" t="s">
         <v>10</v>
       </c>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
     </row>
     <row r="16" spans="1:62">
       <c r="A16" t="s">
@@ -1309,14 +1355,11 @@
       <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="X17" s="4"/>
     </row>
     <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>47</v>
       </c>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:38">
       <c r="A19" t="s">
@@ -1342,6 +1385,11 @@
       <c r="K21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
     </row>
     <row r="22" spans="1:38">
       <c r="A22" t="s">
@@ -1381,6 +1429,7 @@
       <c r="A27" t="s">
         <v>36</v>
       </c>
+      <c r="Y27" s="4"/>
       <c r="AG27" s="4"/>
     </row>
     <row r="28" spans="1:38">

</xml_diff>

<commit_message>
- Create CSButton component to be added to menus - Fully implement button display, with borders and text - Add GridBagLayout to menus - Create buttons to be added to the gridbaylayout and be displayed
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Analysis</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t xml:space="preserve">    UI Wireframes</t>
-  </si>
-  <si>
-    <t>d</t>
   </si>
   <si>
     <t xml:space="preserve">    Neural Net Design</t>
@@ -303,8 +300,26 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,7 +515,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -592,6 +607,15 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -683,6 +707,15 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1015,7 +1048,7 @@
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1025,7 +1058,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3">
         <v>1</v>
@@ -1303,14 +1336,14 @@
     </row>
     <row r="10" spans="1:62">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:62">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1331,7 +1364,7 @@
     </row>
     <row r="14" spans="1:62">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -1345,28 +1378,28 @@
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
+      <c r="AA15" s="4"/>
+      <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:62">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:38">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:38">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:38">
       <c r="A20" t="s">
@@ -1379,9 +1412,7 @@
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="D21" s="4"/>
       <c r="K21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
@@ -1390,6 +1421,10 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
       <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:38">
       <c r="A22" t="s">
@@ -1399,25 +1434,25 @@
     </row>
     <row r="23" spans="1:38">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:38">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T24" s="4"/>
     </row>
     <row r="25" spans="1:38">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L25" s="4"/>
       <c r="AE25" s="4"/>
     </row>
     <row r="26" spans="1:38">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
@@ -1427,54 +1462,54 @@
     </row>
     <row r="27" spans="1:38">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y27" s="4"/>
       <c r="AG27" s="4"/>
     </row>
     <row r="28" spans="1:38">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH28" s="4"/>
     </row>
     <row r="29" spans="1:38">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AI29" s="4"/>
     </row>
     <row r="30" spans="1:38">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AJ30" s="4"/>
     </row>
     <row r="31" spans="1:38">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AK31" s="4"/>
     </row>
     <row r="32" spans="1:38">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL32" s="4"/>
     </row>
     <row r="33" spans="1:59">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:59">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:59">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:59">
@@ -1524,14 +1559,14 @@
     </row>
     <row r="43" spans="1:59">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AQ43" s="4"/>
       <c r="AR43" s="4"/>
     </row>
     <row r="44" spans="1:59">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS44" s="4"/>
       <c r="AT44" s="4"/>

</xml_diff>

<commit_message>
Vertically Centred Textboxes and Beautification
-Change word wrap algorithm so that it can vertically centre the text
-Make UI tweaks to improve looks
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13128E35-6F1B-43D0-955C-8B37E7F778A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14540" yWindow="0" windowWidth="23760" windowHeight="19980" tabRatio="500"/>
+    <workbookView xWindow="58530" yWindow="1050" windowWidth="18000" windowHeight="13185" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -744,6 +750,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1068,20 +1082,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+      <selection activeCell="Z27" sqref="Z27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
-    <col min="25" max="25" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1">
+    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1269,13 +1283,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1288,7 +1302,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1314,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1312,7 +1326,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1326,7 +1340,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1340,7 +1354,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1352,21 +1366,21 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1374,12 +1388,12 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1387,7 +1401,7 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1397,7 +1411,7 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1408,34 +1422,35 @@
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
       <c r="AE15" s="4"/>
-    </row>
-    <row r="16" spans="1:62">
+      <c r="AF15" s="4"/>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1455,30 +1470,30 @@
       <c r="AC21" s="4"/>
       <c r="AD21" s="4"/>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="AD22" s="1"/>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="T24" s="4"/>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1486,115 +1501,111 @@
       <c r="V26" s="4"/>
       <c r="W26" s="7"/>
       <c r="X26" s="4"/>
-      <c r="AF26" s="4"/>
-    </row>
-    <row r="27" spans="1:38">
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="Y27">
-        <v>2019</v>
-      </c>
       <c r="AG27" s="4"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
       <c r="AH28" s="4"/>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="AI29" s="4"/>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="AJ30" s="4"/>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="AK31" s="4"/>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="AL32" s="4"/>
     </row>
-    <row r="33" spans="1:59">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="AM36" s="4"/>
       <c r="AN36" s="4"/>
     </row>
-    <row r="37" spans="1:59">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="AO38" s="4"/>
       <c r="AP38" s="4"/>
     </row>
-    <row r="39" spans="1:59">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="AO39" s="4"/>
       <c r="AP39" s="4"/>
     </row>
-    <row r="40" spans="1:59">
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="AO40" s="4"/>
       <c r="AP40" s="4"/>
     </row>
-    <row r="41" spans="1:59">
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="AO41" s="4"/>
       <c r="AP41" s="4"/>
     </row>
-    <row r="42" spans="1:59">
+    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="AQ43" s="4"/>
       <c r="AR43" s="4"/>
     </row>
-    <row r="44" spans="1:59">
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1603,7 +1614,7 @@
       <c r="AU44" s="4"/>
       <c r="AV44" s="4"/>
     </row>
-    <row r="45" spans="1:59">
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1618,65 +1629,65 @@
       <c r="BE45" s="4"/>
       <c r="BF45" s="4"/>
     </row>
-    <row r="46" spans="1:59">
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="BG47" s="4"/>
     </row>
-    <row r="48" spans="1:59">
+    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="BG48" s="4"/>
     </row>
-    <row r="49" spans="1:62">
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="BH49" s="4"/>
     </row>
-    <row r="50" spans="1:62">
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
       <c r="BI50" s="4"/>
     </row>
-    <row r="51" spans="1:62">
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="BJ52" s="4"/>
     </row>
-    <row r="53" spans="1:62">
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="BJ53" s="4"/>
     </row>
-    <row r="54" spans="1:62">
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="BJ54" s="4"/>
     </row>
-    <row r="55" spans="1:62">
+    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="BJ55" s="4"/>
     </row>
-    <row r="56" spans="1:62">
+    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Neural Framework for Creature Class
-Add creature class
-Give it neural framework instance variables
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F1E75-B5D1-4B08-8798-CBDBB86C635B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="24240" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -515,16 +521,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="213">
@@ -1076,612 +1079,578 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AF15" sqref="AF15"/>
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>7</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>10</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>12</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="2">
         <v>13</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="2">
         <v>14</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="2">
         <v>15</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q1" s="2">
         <v>16</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R1" s="2">
         <v>17</v>
       </c>
-      <c r="S1" s="3">
+      <c r="S1" s="2">
         <v>18</v>
       </c>
-      <c r="T1" s="3">
+      <c r="T1" s="2">
         <v>19</v>
       </c>
-      <c r="U1" s="3">
+      <c r="U1" s="2">
         <v>20</v>
       </c>
-      <c r="V1" s="3">
+      <c r="V1" s="2">
         <v>21</v>
       </c>
-      <c r="W1" s="3">
+      <c r="W1" s="2">
         <v>22</v>
       </c>
-      <c r="X1" s="3">
+      <c r="X1" s="2">
         <v>23</v>
       </c>
-      <c r="Y1" s="3">
+      <c r="Y1" s="2">
         <v>24</v>
       </c>
-      <c r="Z1" s="3">
+      <c r="Z1" s="2">
         <v>25</v>
       </c>
-      <c r="AA1" s="3">
+      <c r="AA1" s="2">
         <v>26</v>
       </c>
-      <c r="AB1" s="3">
+      <c r="AB1" s="2">
         <v>27</v>
       </c>
-      <c r="AC1" s="3">
+      <c r="AC1" s="2">
         <v>28</v>
       </c>
-      <c r="AD1" s="3">
+      <c r="AD1" s="2">
         <v>29</v>
       </c>
-      <c r="AE1" s="3">
+      <c r="AE1" s="2">
         <v>30</v>
       </c>
-      <c r="AF1" s="3">
+      <c r="AF1" s="2">
         <v>31</v>
       </c>
-      <c r="AG1" s="3">
+      <c r="AG1" s="2">
         <v>32</v>
       </c>
-      <c r="AH1" s="3">
+      <c r="AH1" s="2">
         <v>33</v>
       </c>
-      <c r="AI1" s="3">
+      <c r="AI1" s="2">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3">
+      <c r="AJ1" s="2">
         <v>35</v>
       </c>
-      <c r="AK1" s="3">
+      <c r="AK1" s="2">
         <v>36</v>
       </c>
-      <c r="AL1" s="3">
+      <c r="AL1" s="2">
         <v>37</v>
       </c>
-      <c r="AM1" s="3">
+      <c r="AM1" s="2">
         <v>38</v>
       </c>
-      <c r="AN1" s="3">
+      <c r="AN1" s="2">
         <v>39</v>
       </c>
-      <c r="AO1" s="3">
+      <c r="AO1" s="2">
         <v>40</v>
       </c>
-      <c r="AP1" s="3">
+      <c r="AP1" s="2">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3">
+      <c r="AQ1" s="2">
         <v>42</v>
       </c>
-      <c r="AR1" s="3">
+      <c r="AR1" s="2">
         <v>43</v>
       </c>
-      <c r="AS1" s="3">
+      <c r="AS1" s="2">
         <v>44</v>
       </c>
-      <c r="AT1" s="3">
+      <c r="AT1" s="2">
         <v>45</v>
       </c>
-      <c r="AU1" s="3">
+      <c r="AU1" s="2">
         <v>46</v>
       </c>
-      <c r="AV1" s="3">
+      <c r="AV1" s="2">
         <v>47</v>
       </c>
-      <c r="AW1" s="3">
+      <c r="AW1" s="2">
         <v>48</v>
       </c>
-      <c r="AX1" s="3">
+      <c r="AX1" s="2">
         <v>49</v>
       </c>
-      <c r="AY1" s="3">
+      <c r="AY1" s="2">
         <v>50</v>
       </c>
-      <c r="AZ1" s="3">
+      <c r="AZ1" s="2">
         <v>51</v>
       </c>
-      <c r="BA1" s="3">
+      <c r="BA1" s="2">
         <v>52</v>
       </c>
-      <c r="BB1" s="3">
+      <c r="BB1" s="2">
         <v>53</v>
       </c>
-      <c r="BC1" s="3">
+      <c r="BC1" s="2">
         <v>54</v>
       </c>
-      <c r="BD1" s="3">
+      <c r="BD1" s="2">
         <v>55</v>
       </c>
-      <c r="BE1" s="3">
+      <c r="BE1" s="2">
         <v>56</v>
       </c>
-      <c r="BF1" s="3">
+      <c r="BF1" s="2">
         <v>57</v>
       </c>
-      <c r="BG1" s="3">
+      <c r="BG1" s="2">
         <v>58</v>
       </c>
-      <c r="BH1" s="3">
+      <c r="BH1" s="2">
         <v>59</v>
       </c>
-      <c r="BI1" s="3">
+      <c r="BI1" s="2">
         <v>60</v>
       </c>
-      <c r="BJ1" s="3">
+      <c r="BJ1" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:62">
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:62">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:62">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:62">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:62">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:62">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:62">
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-    </row>
-    <row r="10" spans="1:62">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:62">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:62">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-    </row>
-    <row r="14" spans="1:62">
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-    </row>
-    <row r="15" spans="1:62">
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-    </row>
-    <row r="16" spans="1:62">
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:38">
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-    </row>
-    <row r="22" spans="1:38">
+      <c r="D21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="AD22" s="1"/>
-    </row>
-    <row r="23" spans="1:38">
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
-      <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="1:38">
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:38">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="4"/>
-    </row>
-    <row r="27" spans="1:38">
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="AG27" s="4"/>
-    </row>
-    <row r="28" spans="1:38">
+      <c r="AG27" s="3"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="AH28" s="4"/>
-    </row>
-    <row r="29" spans="1:38">
+      <c r="AH28" s="3"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="AI29" s="4"/>
-    </row>
-    <row r="30" spans="1:38">
+      <c r="AI29" s="3"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="AJ30" s="4"/>
-    </row>
-    <row r="31" spans="1:38">
+      <c r="AJ30" s="3"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
-      <c r="AK31" s="4"/>
-    </row>
-    <row r="32" spans="1:38">
+      <c r="AK31" s="3"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
-      <c r="AL32" s="4"/>
-    </row>
-    <row r="33" spans="1:59">
+      <c r="AL32" s="3"/>
+    </row>
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="AM36" s="4"/>
-      <c r="AN36" s="4"/>
-    </row>
-    <row r="37" spans="1:59">
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="3"/>
+    </row>
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
-      <c r="AO38" s="4"/>
-      <c r="AP38" s="4"/>
-    </row>
-    <row r="39" spans="1:59">
+      <c r="AO38" s="3"/>
+      <c r="AP38" s="3"/>
+    </row>
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
-      <c r="AO39" s="4"/>
-      <c r="AP39" s="4"/>
-    </row>
-    <row r="40" spans="1:59">
+      <c r="AO39" s="3"/>
+      <c r="AP39" s="3"/>
+    </row>
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
-      <c r="AO40" s="4"/>
-      <c r="AP40" s="4"/>
-    </row>
-    <row r="41" spans="1:59">
+      <c r="AO40" s="3"/>
+      <c r="AP40" s="3"/>
+    </row>
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
-      <c r="AO41" s="4"/>
-      <c r="AP41" s="4"/>
-    </row>
-    <row r="42" spans="1:59">
+      <c r="AO41" s="3"/>
+      <c r="AP41" s="3"/>
+    </row>
+    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="AQ43" s="4"/>
-      <c r="AR43" s="4"/>
-    </row>
-    <row r="44" spans="1:59">
+      <c r="AQ43" s="3"/>
+      <c r="AR43" s="3"/>
+    </row>
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="AS44" s="4"/>
-      <c r="AT44" s="4"/>
-      <c r="AU44" s="4"/>
-      <c r="AV44" s="4"/>
-    </row>
-    <row r="45" spans="1:59">
+      <c r="AS44" s="3"/>
+      <c r="AT44" s="3"/>
+      <c r="AU44" s="3"/>
+      <c r="AV44" s="3"/>
+    </row>
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
-      <c r="AW45" s="4"/>
-      <c r="AX45" s="4"/>
-      <c r="AY45" s="4"/>
-      <c r="AZ45" s="4"/>
-      <c r="BA45" s="4"/>
-      <c r="BB45" s="4"/>
-      <c r="BC45" s="4"/>
-      <c r="BD45" s="4"/>
-      <c r="BE45" s="4"/>
-      <c r="BF45" s="4"/>
-    </row>
-    <row r="46" spans="1:59">
+      <c r="AW45" s="3"/>
+      <c r="AX45" s="3"/>
+      <c r="AY45" s="3"/>
+      <c r="AZ45" s="3"/>
+      <c r="BA45" s="3"/>
+      <c r="BB45" s="3"/>
+      <c r="BC45" s="3"/>
+      <c r="BD45" s="3"/>
+      <c r="BE45" s="3"/>
+      <c r="BF45" s="3"/>
+    </row>
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
-      <c r="BG47" s="4"/>
-    </row>
-    <row r="48" spans="1:59">
+      <c r="BG47" s="3"/>
+    </row>
+    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
-      <c r="BG48" s="4"/>
-    </row>
-    <row r="49" spans="1:62">
+      <c r="BG48" s="3"/>
+    </row>
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
-      <c r="BH49" s="4"/>
-    </row>
-    <row r="50" spans="1:62">
+      <c r="BH49" s="3"/>
+    </row>
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="BI50" s="4"/>
-    </row>
-    <row r="51" spans="1:62">
+      <c r="BI50" s="3"/>
+    </row>
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
-      <c r="BJ52" s="4"/>
-    </row>
-    <row r="53" spans="1:62">
+      <c r="BJ52" s="3"/>
+    </row>
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
-      <c r="BJ53" s="4"/>
-    </row>
-    <row r="54" spans="1:62">
+      <c r="BJ53" s="3"/>
+    </row>
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
-      <c r="BJ54" s="4"/>
-    </row>
-    <row r="55" spans="1:62">
+      <c r="BJ54" s="3"/>
+    </row>
+    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
-      <c r="BJ55" s="4"/>
-    </row>
-    <row r="56" spans="1:62">
+      <c r="BJ55" s="3"/>
+    </row>
+    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Creature can see food pellets, but in both directions
-Implement creatures seeing food pellets
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F1E75-B5D1-4B08-8798-CBDBB86C635B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="24240" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -306,8 +300,12 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="213">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -530,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="213">
+  <cellStyles count="217">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -637,6 +635,8 @@
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -743,6 +743,8 @@
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1079,20 +1081,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1280,32 +1282,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1319,33 +1321,33 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1353,12 +1355,12 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1366,7 +1368,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1376,7 +1378,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1389,32 +1391,34 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+    </row>
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1434,29 +1438,29 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1465,110 +1469,109 @@
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="AH28" s="3"/>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="AJ30" s="3"/>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="AK31" s="3"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:59">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:59">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:59">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:59">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="AM36" s="3"/>
       <c r="AN36" s="3"/>
     </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:59">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:59">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="AO38" s="3"/>
       <c r="AP38" s="3"/>
     </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:59">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:59">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:59">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
     </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:59">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:59">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
     </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:59">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1577,7 +1580,7 @@
       <c r="AU44" s="3"/>
       <c r="AV44" s="3"/>
     </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:59">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1592,65 +1595,65 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:59">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:59">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="BG47" s="3"/>
     </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:59">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
-    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:62">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="BH49" s="3"/>
     </row>
-    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:62">
       <c r="A50" t="s">
         <v>23</v>
       </c>
       <c r="BI50" s="3"/>
     </row>
-    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:62">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:62">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="BJ52" s="3"/>
     </row>
-    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:62">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
-    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:62">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
-    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:62">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="BJ55" s="3"/>
     </row>
-    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:62">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Creature's seeing food pellets (proper) + Number tweaks
-Alter algorithm for seeing creatures so that only ones in front can be seen.
-Increase tick time by factor of 10, then tweak per-tick numbers to balance out
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956ED221-00F9-44CE-919D-663AA4CA8E92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="24240" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1081,20 +1087,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AI16" sqref="AI16"/>
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1">
+    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1282,32 +1288,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1321,33 +1327,33 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1355,12 +1361,12 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1368,7 +1374,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1378,7 +1384,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1391,34 +1397,35 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:62">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
-    </row>
-    <row r="17" spans="1:38">
+      <c r="AJ16" s="3"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1438,29 +1445,29 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1469,109 +1476,109 @@
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="AI29" s="3"/>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="AJ30" s="3"/>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="AK31" s="3"/>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="1:59">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="AM36" s="3"/>
       <c r="AN36" s="3"/>
     </row>
-    <row r="37" spans="1:59">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="AO38" s="3"/>
       <c r="AP38" s="3"/>
     </row>
-    <row r="39" spans="1:59">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
-    <row r="40" spans="1:59">
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
-    <row r="41" spans="1:59">
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
     </row>
-    <row r="42" spans="1:59">
+    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
     </row>
-    <row r="44" spans="1:59">
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1580,7 +1587,7 @@
       <c r="AU44" s="3"/>
       <c r="AV44" s="3"/>
     </row>
-    <row r="45" spans="1:59">
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1595,65 +1602,65 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="1:59">
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="BG47" s="3"/>
     </row>
-    <row r="48" spans="1:59">
+    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
-    <row r="49" spans="1:62">
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="BH49" s="3"/>
     </row>
-    <row r="50" spans="1:62">
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
       <c r="BI50" s="3"/>
     </row>
-    <row r="51" spans="1:62">
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="BJ52" s="3"/>
     </row>
-    <row r="53" spans="1:62">
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
-    <row r="54" spans="1:62">
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
-    <row r="55" spans="1:62">
+    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="BJ55" s="3"/>
     </row>
-    <row r="56" spans="1:62">
+    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Partially completed mutation for synching
-Add generations mutating half of their creatures
-Add creatures mutating random nodes
-Partially finish mutating nodes
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956ED221-00F9-44CE-919D-663AA4CA8E92}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="24240" windowHeight="18240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -306,8 +300,26 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="217">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -534,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="217">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -643,6 +655,15 @@
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -751,6 +772,15 @@
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1087,20 +1117,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AJ16" sqref="AJ16"/>
+      <selection activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1288,32 +1318,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1327,33 +1357,33 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1361,12 +1391,12 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1404,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1384,7 +1414,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1397,35 +1427,36 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AK16" s="3"/>
+    </row>
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1445,29 +1476,29 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1476,109 +1507,110 @@
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+    </row>
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="AI29" s="3"/>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="AJ30" s="3"/>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
         <v>39</v>
       </c>
-      <c r="AK31" s="3"/>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="AL32" s="3"/>
     </row>
-    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:59">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:59">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:59">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:59">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="AM36" s="3"/>
       <c r="AN36" s="3"/>
     </row>
-    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:59">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:59">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="AO38" s="3"/>
       <c r="AP38" s="3"/>
     </row>
-    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:59">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
-    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:59">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
-    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:59">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
     </row>
-    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:59">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:59">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
     </row>
-    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:59">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1587,7 +1619,7 @@
       <c r="AU44" s="3"/>
       <c r="AV44" s="3"/>
     </row>
-    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:59">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1602,65 +1634,65 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:59">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:59">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="BG47" s="3"/>
     </row>
-    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:59">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
-    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:62">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="BH49" s="3"/>
     </row>
-    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:62">
       <c r="A50" t="s">
         <v>23</v>
       </c>
       <c r="BI50" s="3"/>
     </row>
-    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:62">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:62">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="BJ52" s="3"/>
     </row>
-    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:62">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
-    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:62">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
-    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:62">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="BJ55" s="3"/>
     </row>
-    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:62">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Creatures and Food do not spawn on top of one another
-When spawning food, it is checked whether or not it will spawn on top of other bits of food
-When spawning creatures, it is checked whether they will be near other creatures or food
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E808C98-A39A-43DE-A60C-DD6EF88DD379}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="58530" yWindow="1050" windowWidth="18000" windowHeight="13185" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -209,7 +215,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1134,21 +1140,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AM28" sqref="AM28"/>
+      <selection activeCell="AN16" sqref="AN16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1">
+    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -1336,32 +1342,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1375,33 +1381,33 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -1409,12 +1415,12 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1422,7 +1428,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1432,7 +1438,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1445,7 +1451,7 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:62">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1455,28 +1461,29 @@
       <c r="AK16" s="3"/>
       <c r="AL16" s="5"/>
       <c r="AM16" s="5"/>
-    </row>
-    <row r="17" spans="1:39">
+      <c r="AN16" s="5"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1496,29 +1503,29 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1527,13 +1534,13 @@
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1543,94 +1550,94 @@
       <c r="AK28" s="5"/>
       <c r="AM28" s="5"/>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:59">
+    <row r="33" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:59">
+    <row r="34" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:59">
+    <row r="35" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:59">
+    <row r="36" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>28</v>
       </c>
       <c r="AM36" s="3"/>
       <c r="AN36" s="3"/>
     </row>
-    <row r="37" spans="1:59">
+    <row r="37" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:59">
+    <row r="38" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="AO38" s="3"/>
       <c r="AP38" s="3"/>
     </row>
-    <row r="39" spans="1:59">
+    <row r="39" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
-    <row r="40" spans="1:59">
+    <row r="40" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
-    <row r="41" spans="1:59">
+    <row r="41" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
     </row>
-    <row r="42" spans="1:59">
+    <row r="42" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:59">
+    <row r="43" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="3"/>
     </row>
-    <row r="44" spans="1:59">
+    <row r="44" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -1639,7 +1646,7 @@
       <c r="AU44" s="3"/>
       <c r="AV44" s="3"/>
     </row>
-    <row r="45" spans="1:59">
+    <row r="45" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -1654,65 +1661,65 @@
       <c r="BE45" s="3"/>
       <c r="BF45" s="3"/>
     </row>
-    <row r="46" spans="1:59">
+    <row r="46" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:59">
+    <row r="47" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
       <c r="BG47" s="3"/>
     </row>
-    <row r="48" spans="1:59">
+    <row r="48" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>19</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
-    <row r="49" spans="1:62">
+    <row r="49" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>20</v>
       </c>
       <c r="BH49" s="3"/>
     </row>
-    <row r="50" spans="1:62">
+    <row r="50" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
       <c r="BI50" s="3"/>
     </row>
-    <row r="51" spans="1:62">
+    <row r="51" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:62">
+    <row r="52" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>15</v>
       </c>
       <c r="BJ52" s="3"/>
     </row>
-    <row r="53" spans="1:62">
+    <row r="53" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
-    <row r="54" spans="1:62">
+    <row r="54" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>17</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
-    <row r="55" spans="1:62">
+    <row r="55" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="BJ55" s="3"/>
     </row>
-    <row r="56" spans="1:62">
+    <row r="56" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Fixed error with generations carrying on to the next
-Alter algorithm for creatting a new generation based on the previous
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Analysis</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">        Highest Food Graph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        View Previous Generation</t>
   </si>
 </sst>
 </file>
@@ -300,8 +303,16 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="247">
+  <cellStyleXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -559,7 +570,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="247">
+  <cellStyles count="255">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -683,6 +694,10 @@
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -806,6 +821,10 @@
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1143,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ56"/>
+  <dimension ref="A1:BJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AQ30" sqref="AQ30"/>
+      <selection activeCell="AP31" sqref="AP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1570,165 +1589,171 @@
     </row>
     <row r="31" spans="1:42">
       <c r="A31" t="s">
-        <v>38</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="AP31" s="5"/>
     </row>
     <row r="32" spans="1:42">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:59">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:59">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:59">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:59">
       <c r="A36" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM36" s="3"/>
-      <c r="AN36" s="3"/>
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="1:59">
       <c r="A37" t="s">
-        <v>8</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
     </row>
     <row r="38" spans="1:59">
       <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO38" s="3"/>
-      <c r="AP38" s="3"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="1:59">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
     <row r="40" spans="1:59">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
     <row r="41" spans="1:59">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
     </row>
     <row r="42" spans="1:59">
       <c r="A42" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="AO42" s="3"/>
+      <c r="AP42" s="3"/>
     </row>
     <row r="43" spans="1:59">
       <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ43" s="3"/>
-      <c r="AR43" s="3"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="44" spans="1:59">
       <c r="A44" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS44" s="3"/>
-      <c r="AT44" s="3"/>
-      <c r="AU44" s="3"/>
-      <c r="AV44" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="AQ44" s="3"/>
+      <c r="AR44" s="3"/>
     </row>
     <row r="45" spans="1:59">
       <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW45" s="3"/>
-      <c r="AX45" s="3"/>
-      <c r="AY45" s="3"/>
-      <c r="AZ45" s="3"/>
-      <c r="BA45" s="3"/>
-      <c r="BB45" s="3"/>
-      <c r="BC45" s="3"/>
-      <c r="BD45" s="3"/>
-      <c r="BE45" s="3"/>
-      <c r="BF45" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="AS45" s="3"/>
+      <c r="AT45" s="3"/>
+      <c r="AU45" s="3"/>
+      <c r="AV45" s="3"/>
     </row>
     <row r="46" spans="1:59">
       <c r="A46" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="AW46" s="3"/>
+      <c r="AX46" s="3"/>
+      <c r="AY46" s="3"/>
+      <c r="AZ46" s="3"/>
+      <c r="BA46" s="3"/>
+      <c r="BB46" s="3"/>
+      <c r="BC46" s="3"/>
+      <c r="BD46" s="3"/>
+      <c r="BE46" s="3"/>
+      <c r="BF46" s="3"/>
     </row>
     <row r="47" spans="1:59">
       <c r="A47" t="s">
-        <v>22</v>
-      </c>
-      <c r="BG47" s="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="48" spans="1:59">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
     <row r="49" spans="1:62">
       <c r="A49" t="s">
-        <v>20</v>
-      </c>
-      <c r="BH49" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="BG49" s="3"/>
     </row>
     <row r="50" spans="1:62">
       <c r="A50" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI50" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="BH50" s="3"/>
     </row>
     <row r="51" spans="1:62">
       <c r="A51" t="s">
-        <v>26</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="BI51" s="3"/>
     </row>
     <row r="52" spans="1:62">
       <c r="A52" t="s">
-        <v>15</v>
-      </c>
-      <c r="BJ52" s="3"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="53" spans="1:62">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
     <row r="54" spans="1:62">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
     <row r="55" spans="1:62">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="BJ55" s="3"/>
     </row>
     <row r="56" spans="1:62">
       <c r="A56" t="s">
+        <v>18</v>
+      </c>
+      <c r="BJ56" s="3"/>
+    </row>
+    <row r="57" spans="1:62">
+      <c r="A57" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Give Creatures Random Names
-Download list of names
-When a creature is created, give it a random first name
-When a creature is created, give it a surname based on it's parent
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>Analysis</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">    Fast Generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Creature Cannabalism</t>
   </si>
   <si>
     <t xml:space="preserve">    Creature Names</t>
@@ -303,8 +300,10 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="255">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -570,7 +569,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="255">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -698,6 +697,7 @@
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -825,6 +825,7 @@
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1162,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ57"/>
+  <dimension ref="A1:BJ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AP31" sqref="AP31"/>
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1177,7 +1178,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="2">
         <v>1</v>
@@ -1404,7 +1405,7 @@
     </row>
     <row r="7" spans="1:62">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1416,21 +1417,21 @@
     </row>
     <row r="9" spans="1:62">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
     <row r="10" spans="1:62">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:62">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1451,7 +1452,7 @@
     </row>
     <row r="14" spans="1:62">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
@@ -1484,116 +1485,117 @@
       <c r="AM16" s="5"/>
       <c r="AN16" s="5"/>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:43">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="AO17" s="5"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:43">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AO18" s="5"/>
       <c r="AP18" s="5"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:43">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:42">
+      <c r="AQ19" s="5"/>
+    </row>
+    <row r="20" spans="1:43">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:42">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="1:43">
       <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43">
       <c r="A22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43">
       <c r="A23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:42">
+        <v>46</v>
+      </c>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:43">
       <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="1:42">
+        <v>32</v>
+      </c>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:43">
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:42">
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="3"/>
+    </row>
+    <row r="26" spans="1:43">
       <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="U26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="3"/>
-    </row>
-    <row r="27" spans="1:42">
+      <c r="AG26" s="3"/>
+    </row>
+    <row r="27" spans="1:43">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="AG27" s="3"/>
-    </row>
-    <row r="28" spans="1:42">
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AO27" s="5"/>
+    </row>
+    <row r="28" spans="1:43">
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="AH28" s="3"/>
-      <c r="AI28" s="3"/>
-      <c r="AJ28" s="3"/>
-      <c r="AK28" s="5"/>
-      <c r="AM28" s="5"/>
       <c r="AO28" s="5"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:43">
       <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO29" s="5"/>
-    </row>
-    <row r="30" spans="1:42">
+        <v>50</v>
+      </c>
+      <c r="AP29" s="5"/>
+    </row>
+    <row r="30" spans="1:43">
       <c r="A30" t="s">
         <v>51</v>
       </c>
       <c r="AP30" s="5"/>
     </row>
-    <row r="31" spans="1:42">
+    <row r="31" spans="1:43">
       <c r="A31" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP31" s="5"/>
-    </row>
-    <row r="32" spans="1:42">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:43">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1610,25 +1612,27 @@
     </row>
     <row r="35" spans="1:59">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:59">
       <c r="A36" t="s">
-        <v>43</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="3"/>
     </row>
     <row r="37" spans="1:59">
       <c r="A37" t="s">
-        <v>28</v>
-      </c>
-      <c r="AM37" s="3"/>
-      <c r="AN37" s="3"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="38" spans="1:59">
       <c r="A38" t="s">
-        <v>8</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="AO38" s="3"/>
+      <c r="AP38" s="3"/>
     </row>
     <row r="39" spans="1:59">
       <c r="A39" t="s">
@@ -1653,55 +1657,54 @@
     </row>
     <row r="42" spans="1:59">
       <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="AO42" s="3"/>
-      <c r="AP42" s="3"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="43" spans="1:59">
       <c r="A43" t="s">
-        <v>24</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="AQ43" s="3"/>
+      <c r="AR43" s="3"/>
     </row>
     <row r="44" spans="1:59">
       <c r="A44" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ44" s="3"/>
-      <c r="AR44" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="AS44" s="3"/>
+      <c r="AT44" s="3"/>
+      <c r="AU44" s="3"/>
+      <c r="AV44" s="3"/>
     </row>
     <row r="45" spans="1:59">
       <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS45" s="3"/>
-      <c r="AT45" s="3"/>
-      <c r="AU45" s="3"/>
-      <c r="AV45" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="AW45" s="3"/>
+      <c r="AX45" s="3"/>
+      <c r="AY45" s="3"/>
+      <c r="AZ45" s="3"/>
+      <c r="BA45" s="3"/>
+      <c r="BB45" s="3"/>
+      <c r="BC45" s="3"/>
+      <c r="BD45" s="3"/>
+      <c r="BE45" s="3"/>
+      <c r="BF45" s="3"/>
     </row>
     <row r="46" spans="1:59">
       <c r="A46" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW46" s="3"/>
-      <c r="AX46" s="3"/>
-      <c r="AY46" s="3"/>
-      <c r="AZ46" s="3"/>
-      <c r="BA46" s="3"/>
-      <c r="BB46" s="3"/>
-      <c r="BC46" s="3"/>
-      <c r="BD46" s="3"/>
-      <c r="BE46" s="3"/>
-      <c r="BF46" s="3"/>
+        <v>24</v>
+      </c>
     </row>
     <row r="47" spans="1:59">
       <c r="A47" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="BG47" s="3"/>
     </row>
     <row r="48" spans="1:59">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="BG48" s="3"/>
     </row>
@@ -1709,24 +1712,24 @@
       <c r="A49" t="s">
         <v>19</v>
       </c>
-      <c r="BG49" s="3"/>
+      <c r="BH49" s="3"/>
     </row>
     <row r="50" spans="1:62">
       <c r="A50" t="s">
-        <v>20</v>
-      </c>
-      <c r="BH50" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="BI50" s="3"/>
     </row>
     <row r="51" spans="1:62">
       <c r="A51" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI51" s="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="52" spans="1:62">
       <c r="A52" t="s">
-        <v>26</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="BJ52" s="3"/>
     </row>
     <row r="53" spans="1:62">
       <c r="A53" t="s">
@@ -1748,13 +1751,7 @@
     </row>
     <row r="56" spans="1:62">
       <c r="A56" t="s">
-        <v>18</v>
-      </c>
-      <c r="BJ56" s="3"/>
-    </row>
-    <row r="57" spans="1:62">
-      <c r="A57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning up record of progress et al
-Fix some errors in record of progress
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Analysis</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t xml:space="preserve">        View Previous Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Creature learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Creature learning</t>
   </si>
 </sst>
 </file>
@@ -297,8 +303,20 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="269">
+  <cellStyleXfs count="281">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -578,7 +596,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="269">
+  <cellStyles count="281">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -713,6 +731,12 @@
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -847,6 +871,12 @@
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1184,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ55"/>
+  <dimension ref="A1:BJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AS31" sqref="AS31"/>
+      <selection activeCell="AV33" sqref="AV33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1506,20 +1536,20 @@
       <c r="AM16" s="5"/>
       <c r="AN16" s="5"/>
     </row>
-    <row r="17" spans="1:45">
+    <row r="17" spans="1:47">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="AO17" s="5"/>
     </row>
-    <row r="18" spans="1:45">
+    <row r="18" spans="1:47">
       <c r="A18" t="s">
         <v>47</v>
       </c>
       <c r="AO18" s="5"/>
       <c r="AP18" s="5"/>
     </row>
-    <row r="19" spans="1:45">
+    <row r="19" spans="1:47">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1527,249 +1557,261 @@
       <c r="AR19" s="5"/>
       <c r="AS19" s="5"/>
     </row>
-    <row r="20" spans="1:45">
+    <row r="20" spans="1:47">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT20" s="5"/>
+      <c r="AU20" s="5"/>
+    </row>
+    <row r="21" spans="1:47">
+      <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:45">
-      <c r="A21" t="s">
+      <c r="D21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:47">
+      <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:45">
-      <c r="A22" t="s">
+    <row r="23" spans="1:47">
+      <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:45">
-      <c r="A23" t="s">
+    <row r="24" spans="1:47">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="1:45">
-      <c r="A24" t="s">
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:47">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:45">
-      <c r="A25" t="s">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:47">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="U25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="3"/>
-    </row>
-    <row r="26" spans="1:45">
-      <c r="A26" t="s">
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="1:47">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="AG26" s="3"/>
-    </row>
-    <row r="27" spans="1:45">
-      <c r="A27" t="s">
+      <c r="AG27" s="3"/>
+    </row>
+    <row r="28" spans="1:47">
+      <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="AH27" s="3"/>
-      <c r="AI27" s="3"/>
-      <c r="AJ27" s="3"/>
-      <c r="AK27" s="5"/>
-      <c r="AM27" s="5"/>
-      <c r="AO27" s="5"/>
-    </row>
-    <row r="28" spans="1:45">
-      <c r="A28" t="s">
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AO28" s="5"/>
+    </row>
+    <row r="29" spans="1:47">
+      <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="AO28" s="5"/>
-    </row>
-    <row r="29" spans="1:45">
-      <c r="A29" t="s">
+      <c r="AO29" s="5"/>
+    </row>
+    <row r="30" spans="1:47">
+      <c r="A30" t="s">
         <v>49</v>
       </c>
-      <c r="AP29" s="5"/>
-    </row>
-    <row r="30" spans="1:45">
-      <c r="A30" t="s">
+      <c r="AP30" s="5"/>
+    </row>
+    <row r="31" spans="1:47">
+      <c r="A31" t="s">
         <v>50</v>
       </c>
-      <c r="AP30" s="5"/>
-    </row>
-    <row r="31" spans="1:45">
-      <c r="A31" t="s">
+      <c r="AP31" s="5"/>
+    </row>
+    <row r="32" spans="1:47">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="AR31" s="5"/>
-    </row>
-    <row r="32" spans="1:45">
-      <c r="A32" t="s">
+      <c r="AR32" s="5"/>
+    </row>
+    <row r="33" spans="1:59">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:59">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:60">
-      <c r="A33" t="s">
+    <row r="35" spans="1:59">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:60">
-      <c r="A34" t="s">
+    <row r="36" spans="1:59">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:60">
-      <c r="A35" t="s">
+    <row r="37" spans="1:59">
+      <c r="A37" t="s">
         <v>27</v>
       </c>
-      <c r="AM35" s="3"/>
-      <c r="AN35" s="3"/>
-    </row>
-    <row r="36" spans="1:60">
-      <c r="A36" t="s">
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="3"/>
+    </row>
+    <row r="38" spans="1:59">
+      <c r="A38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:60">
-      <c r="A37" t="s">
+    <row r="39" spans="1:59">
+      <c r="A39" t="s">
         <v>14</v>
-      </c>
-      <c r="AO37" s="3"/>
-      <c r="AP37" s="3"/>
-    </row>
-    <row r="38" spans="1:60">
-      <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO38" s="3"/>
-      <c r="AP38" s="3"/>
-    </row>
-    <row r="39" spans="1:60">
-      <c r="A39" t="s">
-        <v>16</v>
       </c>
       <c r="AO39" s="3"/>
       <c r="AP39" s="3"/>
     </row>
-    <row r="40" spans="1:60">
+    <row r="40" spans="1:59">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AO40" s="3"/>
       <c r="AP40" s="3"/>
     </row>
-    <row r="41" spans="1:60">
+    <row r="41" spans="1:59">
       <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO41" s="3"/>
+      <c r="AP41" s="3"/>
+    </row>
+    <row r="42" spans="1:59">
+      <c r="A42" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO42" s="3"/>
+      <c r="AP42" s="3"/>
+    </row>
+    <row r="43" spans="1:59">
+      <c r="A43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:60">
-      <c r="A42" t="s">
+    <row r="44" spans="1:59">
+      <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="AQ42" s="3"/>
-      <c r="AR42" s="3"/>
-    </row>
-    <row r="43" spans="1:60">
-      <c r="A43" t="s">
+      <c r="AQ44" s="3"/>
+      <c r="AR44" s="3"/>
+    </row>
+    <row r="45" spans="1:59">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="AS43" s="3"/>
-      <c r="AT43" s="3"/>
-      <c r="AU43" s="3"/>
-      <c r="AV43" s="3"/>
-    </row>
-    <row r="44" spans="1:60">
-      <c r="A44" t="s">
+      <c r="AS45" s="3"/>
+      <c r="AT45" s="3"/>
+      <c r="AU45" s="3"/>
+      <c r="AV45" s="3"/>
+    </row>
+    <row r="46" spans="1:59">
+      <c r="A46" t="s">
         <v>20</v>
       </c>
-      <c r="AW44" s="3"/>
-      <c r="AX44" s="3"/>
-      <c r="AY44" s="3"/>
-      <c r="AZ44" s="3"/>
-      <c r="BA44" s="3"/>
-      <c r="BB44" s="3"/>
-      <c r="BC44" s="3"/>
-      <c r="BD44" s="3"/>
-      <c r="BE44" s="3"/>
-      <c r="BF44" s="3"/>
-    </row>
-    <row r="45" spans="1:60">
-      <c r="A45" t="s">
+      <c r="AW46" s="3"/>
+      <c r="AX46" s="3"/>
+      <c r="AY46" s="3"/>
+      <c r="AZ46" s="3"/>
+      <c r="BA46" s="3"/>
+      <c r="BB46" s="3"/>
+      <c r="BC46" s="3"/>
+      <c r="BD46" s="3"/>
+      <c r="BE46" s="3"/>
+      <c r="BF46" s="3"/>
+    </row>
+    <row r="47" spans="1:59">
+      <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:60">
-      <c r="A46" t="s">
+    <row r="48" spans="1:59">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="BG46" s="3"/>
-    </row>
-    <row r="47" spans="1:60">
-      <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="BG47" s="3"/>
-    </row>
-    <row r="48" spans="1:60">
-      <c r="A48" t="s">
-        <v>19</v>
-      </c>
-      <c r="BH48" s="3"/>
+      <c r="BG48" s="3"/>
     </row>
     <row r="49" spans="1:62">
       <c r="A49" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI49" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="BG49" s="3"/>
     </row>
     <row r="50" spans="1:62">
       <c r="A50" t="s">
-        <v>25</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="BH50" s="3"/>
     </row>
     <row r="51" spans="1:62">
       <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="BJ51" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="BI51" s="3"/>
     </row>
     <row r="52" spans="1:62">
       <c r="A52" t="s">
-        <v>15</v>
-      </c>
-      <c r="BJ52" s="3"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="53" spans="1:62">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BJ53" s="3"/>
     </row>
     <row r="54" spans="1:62">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="BJ54" s="3"/>
     </row>
     <row r="55" spans="1:62">
       <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="BJ55" s="3"/>
+    </row>
+    <row r="56" spans="1:62">
+      <c r="A56" t="s">
+        <v>17</v>
+      </c>
+      <c r="BJ56" s="3"/>
+    </row>
+    <row r="57" spans="1:62">
+      <c r="A57" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fucntionality testing carried out
</commit_message>
<xml_diff>
--- a/Revised Gantt Chart.xlsx
+++ b/Revised Gantt Chart.xlsx
@@ -1,16 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakes\Programming\Java\CreatureSim\CreatureSim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920CAC6C-CAC7-46D5-9570-5E06DEB7E581}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -212,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1213,21 +1225,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BJ57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="AV33" sqref="AV33"/>
+      <selection activeCell="DQ22" sqref="DQ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.125" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.125" customWidth="1"/>
     <col min="25" max="25" width="3.125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="18" customHeight="1">
+    <row r="1" spans="1:62" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1415,32 +1427,32 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:62">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:62">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:62">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1454,33 +1466,33 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:62">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:62">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:62">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:62">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:62">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -1488,12 +1500,12 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:62">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:62">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1501,7 +1513,7 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
     </row>
-    <row r="14" spans="1:62">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1511,7 +1523,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:62">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1523,8 +1535,9 @@
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
-    </row>
-    <row r="16" spans="1:62">
+      <c r="AV15" s="5"/>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1536,35 +1549,36 @@
       <c r="AM16" s="5"/>
       <c r="AN16" s="5"/>
     </row>
-    <row r="17" spans="1:47">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="AO17" s="5"/>
     </row>
-    <row r="18" spans="1:47">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
       <c r="AO18" s="5"/>
       <c r="AP18" s="5"/>
     </row>
-    <row r="19" spans="1:47">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="AQ19" s="5"/>
       <c r="AR19" s="5"/>
       <c r="AS19" s="5"/>
-    </row>
-    <row r="20" spans="1:47">
+      <c r="AW19" s="5"/>
+    </row>
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
       <c r="AT20" s="5"/>
       <c r="AU20" s="5"/>
     </row>
-    <row r="21" spans="1:47">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1584,29 +1598,29 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:47">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:47">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:47">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="T24" s="3"/>
     </row>
-    <row r="25" spans="1:47">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:47">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1615,13 +1629,13 @@
       <c r="W26" s="4"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:47">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:47">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1632,185 +1646,152 @@
       <c r="AM28" s="5"/>
       <c r="AO28" s="5"/>
     </row>
-    <row r="29" spans="1:47">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
       <c r="AO29" s="5"/>
     </row>
-    <row r="30" spans="1:47">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
       <c r="AP30" s="5"/>
     </row>
-    <row r="31" spans="1:47">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
       <c r="AP31" s="5"/>
     </row>
-    <row r="32" spans="1:47">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
       <c r="AR32" s="5"/>
     </row>
-    <row r="33" spans="1:59">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:59">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:59">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:59">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:59">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
-      <c r="AM37" s="3"/>
-      <c r="AN37" s="3"/>
-    </row>
-    <row r="38" spans="1:59">
+    </row>
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:59">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
-      <c r="AO39" s="3"/>
-      <c r="AP39" s="3"/>
-    </row>
-    <row r="40" spans="1:59">
+    </row>
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>15</v>
       </c>
-      <c r="AO40" s="3"/>
-      <c r="AP40" s="3"/>
-    </row>
-    <row r="41" spans="1:59">
+    </row>
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
-      <c r="AO41" s="3"/>
-      <c r="AP41" s="3"/>
-    </row>
-    <row r="42" spans="1:59">
+    </row>
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
-      <c r="AO42" s="3"/>
-      <c r="AP42" s="3"/>
-    </row>
-    <row r="43" spans="1:59">
+    </row>
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:59">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
-      <c r="AQ44" s="3"/>
-      <c r="AR44" s="3"/>
-    </row>
-    <row r="45" spans="1:59">
+      <c r="AS44" s="5"/>
+    </row>
+    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-      <c r="AS45" s="3"/>
-      <c r="AT45" s="3"/>
-      <c r="AU45" s="3"/>
-      <c r="AV45" s="3"/>
-    </row>
-    <row r="46" spans="1:59">
+    </row>
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
-      <c r="AW46" s="3"/>
-      <c r="AX46" s="3"/>
-      <c r="AY46" s="3"/>
-      <c r="AZ46" s="3"/>
-      <c r="BA46" s="3"/>
-      <c r="BB46" s="3"/>
-      <c r="BC46" s="3"/>
-      <c r="BD46" s="3"/>
-      <c r="BE46" s="3"/>
-      <c r="BF46" s="3"/>
-    </row>
-    <row r="47" spans="1:59">
+    </row>
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:59">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="BG48" s="3"/>
-    </row>
-    <row r="49" spans="1:62">
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
-      <c r="BG49" s="3"/>
-    </row>
-    <row r="50" spans="1:62">
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>19</v>
       </c>
-      <c r="BH50" s="3"/>
-    </row>
-    <row r="51" spans="1:62">
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
-      <c r="BI51" s="3"/>
-    </row>
-    <row r="52" spans="1:62">
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:62">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
-      <c r="BJ53" s="3"/>
-    </row>
-    <row r="54" spans="1:62">
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>15</v>
       </c>
-      <c r="BJ54" s="3"/>
-    </row>
-    <row r="55" spans="1:62">
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
-      <c r="BJ55" s="3"/>
-    </row>
-    <row r="56" spans="1:62">
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>17</v>
       </c>
-      <c r="BJ56" s="3"/>
-    </row>
-    <row r="57" spans="1:62">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>26</v>
       </c>

</xml_diff>